<commit_message>
Iniciandi a Ligação com a tabela
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefetrjbr-my.sharepoint.com/personal/08951123960_cefet-rj_br/Documents/Nathan - Faculdade/8° período/EQUIPAMENTOS ELÉTRICOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kramm\OneDrive - cefet-rj.br\Faculdade\01 - Período Atual\Equipamentos\Interface\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{500DA131-89F7-43C2-9D36-0698431F4AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="13" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
   </bookViews>
   <sheets>
     <sheet name="4.23.uni" sheetId="11" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E826B28E-EC7C-4B1D-B269-53FEA7A54F81}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A6DC8A-33F4-4D1E-B104-D261E463BA17}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Iniciando a Ligação com a tabela
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefetrjbr-my.sharepoint.com/personal/08951123960_cefet-rj_br/Documents/Nathan - Faculdade/8° período/EQUIPAMENTOS ELÉTRICOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kramm\OneDrive - cefet-rj.br\Faculdade\01 - Período Atual\Equipamentos\Interface\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{500DA131-89F7-43C2-9D36-0698431F4AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="13" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
   </bookViews>
   <sheets>
     <sheet name="4.23.uni" sheetId="11" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E826B28E-EC7C-4B1D-B269-53FEA7A54F81}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,7 +2888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A6DC8A-33F4-4D1E-B104-D261E463BA17}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Interface de consulta a tabelas 90% Finalizada
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kramm\OneDrive - cefet-rj.br\Faculdade\01 - Período Atual\Equipamentos\Interface\Tabelas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kramm\Desktop\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{500DA131-89F7-43C2-9D36-0698431F4AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37A29C2-D1E4-466C-BB80-1BEF0EE96E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="13" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
   </bookViews>
   <sheets>
     <sheet name="4.23.uni" sheetId="11" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="12">
   <si>
     <t>Seção condutor</t>
   </si>
@@ -89,8 +89,16 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,7 +144,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E826B28E-EC7C-4B1D-B269-53FEA7A54F81}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +477,7 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,8 +508,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -531,8 +543,11 @@
       <c r="J2" s="2">
         <v>2.9262000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.5</v>
       </c>
@@ -563,8 +578,11 @@
       <c r="J3" s="2">
         <v>2.8755000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -595,8 +613,11 @@
       <c r="J4" s="2">
         <v>2.8349000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -627,8 +648,11 @@
       <c r="J5" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -659,8 +683,11 @@
       <c r="J6" s="2">
         <v>2.7639</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
@@ -691,8 +718,11 @@
       <c r="J7" s="2">
         <v>2.7172999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -723,8 +753,11 @@
       <c r="J8" s="2">
         <v>2.6692</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -755,8 +788,11 @@
       <c r="J9" s="2">
         <v>2.6381999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -787,8 +823,11 @@
       <c r="J10" s="2">
         <v>2.5991</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>70</v>
       </c>
@@ -819,8 +858,11 @@
       <c r="J11" s="2">
         <v>2.5680999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>95</v>
       </c>
@@ -851,8 +893,11 @@
       <c r="J12" s="2">
         <v>2.5325000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -883,8 +928,11 @@
       <c r="J13" s="2">
         <v>2.5104000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>150</v>
       </c>
@@ -915,8 +963,11 @@
       <c r="J14" s="2">
         <v>2.4843000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>185</v>
       </c>
@@ -947,8 +998,11 @@
       <c r="J15" s="2">
         <v>2.4594</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>240</v>
       </c>
@@ -979,8 +1033,11 @@
       <c r="J16" s="2">
         <v>2.4312</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>300</v>
       </c>
@@ -1011,8 +1068,11 @@
       <c r="J17" s="2">
         <v>2.4066999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>400</v>
       </c>
@@ -1043,8 +1103,11 @@
       <c r="J18" s="2">
         <v>2.3757000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>500</v>
       </c>
@@ -1075,9 +1138,13 @@
       <c r="J19" s="2">
         <v>2.3491</v>
       </c>
+      <c r="K19" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2888,7 +2955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A6DC8A-33F4-4D1E-B104-D261E463BA17}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -3037,7 +3104,7 @@
       <c r="J4" s="2">
         <v>0.1046</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3363,10 +3430,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EF6948-971C-4BEB-9DF1-7B215B1759C0}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3378,7 +3445,7 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3409,8 +3476,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>25</v>
       </c>
@@ -3441,8 +3511,11 @@
       <c r="J2" s="2">
         <v>2.1718000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>35</v>
       </c>
@@ -3473,8 +3546,11 @@
       <c r="J3" s="2">
         <v>2.1549999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -3505,8 +3581,11 @@
       <c r="J4" s="2">
         <v>2.1419000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>70</v>
       </c>
@@ -3537,8 +3616,11 @@
       <c r="J5" s="2">
         <v>2.1265000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>95</v>
       </c>
@@ -3569,8 +3651,11 @@
       <c r="J6" s="2">
         <v>2.1145999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>120</v>
       </c>
@@ -3601,8 +3686,11 @@
       <c r="J7" s="2">
         <v>2.1038000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>150</v>
       </c>
@@ -3633,8 +3721,11 @@
       <c r="J8" s="2">
         <v>2.0951</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>240</v>
       </c>
@@ -3665,6 +3756,39 @@
       <c r="J9" s="2">
         <v>2.0762</v>
       </c>
+      <c r="K9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3675,7 +3799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F42EEC2-E051-4B8C-898A-18D14D380CE2}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -4362,7 +4486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D903FD3-C7E0-458D-A487-AEC5D0129AB9}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -4734,7 +4858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518857E0-2C2D-4BDA-8E85-FB62541DEF4B}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8:K19"/>
     </sheetView>
   </sheetViews>
@@ -7166,9 +7290,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC86C6A-60BF-4FED-A078-F656B26D8126}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -7531,12 +7655,24 @@
         <v>11</v>
       </c>
     </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EF56198A93F1A44A95BAE701B4EF6ED0" ma:contentTypeVersion="7" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="de71b56f3e2d213272193eb1d6fad728">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5560cc27-b74c-4309-beba-079b2192b5e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e0b56cf1064610ffb0cb8ad42962a7e" ns3:_="">
     <xsd:import namespace="5560cc27-b74c-4309-beba-079b2192b5e3"/>
@@ -7700,15 +7836,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7716,6 +7843,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C2B197-2619-4D79-9DD7-B8B741DC09D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D269DB-F7F0-443B-A4D2-D98356E0AD5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7733,14 +7868,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C2B197-2619-4D79-9DD7-B8B741DC09D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6FD7EE7-48D9-494D-920A-A7144B7109DB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Removendo o bug de Seção de 185 mm2 para os condutores de aluminío
</commit_message>
<xml_diff>
--- a/Tabelas/Tabelas.xlsx
+++ b/Tabelas/Tabelas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kramm\Desktop\Tabelas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kramm\OneDrive - cefet-rj.br\Faculdade\01 - Período Atual\Equipamentos\Interface\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37A29C2-D1E4-466C-BB80-1BEF0EE96E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{D37A29C2-D1E4-466C-BB80-1BEF0EE96E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FB347467-659E-46D4-9BA5-D6B57C973047}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="13" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D0D0BAE2-3AC5-48E7-BC87-84100C0FDB07}"/>
   </bookViews>
   <sheets>
     <sheet name="4.23.uni" sheetId="11" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="12">
   <si>
     <t>Seção condutor</t>
   </si>
@@ -2955,7 +2955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A6DC8A-33F4-4D1E-B104-D261E463BA17}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -3430,10 +3430,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EF6948-971C-4BEB-9DF1-7B215B1759C0}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,41 +3727,73 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>185</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>240</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>332</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>405</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>406</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>359</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>357</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>9.5399999999999999E-2</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="2">
         <v>0.27300000000000002</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J10" s="2">
         <v>2.0762</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K11" s="1"/>
@@ -3779,19 +3811,15 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="7"/>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7664,15 +7692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EF56198A93F1A44A95BAE701B4EF6ED0" ma:contentTypeVersion="7" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="de71b56f3e2d213272193eb1d6fad728">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5560cc27-b74c-4309-beba-079b2192b5e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e0b56cf1064610ffb0cb8ad42962a7e" ns3:_="">
     <xsd:import namespace="5560cc27-b74c-4309-beba-079b2192b5e3"/>
@@ -7836,6 +7855,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7843,14 +7871,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C2B197-2619-4D79-9DD7-B8B741DC09D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D269DB-F7F0-443B-A4D2-D98356E0AD5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7868,6 +7888,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C2B197-2619-4D79-9DD7-B8B741DC09D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6FD7EE7-48D9-494D-920A-A7144B7109DB}">
   <ds:schemaRefs>

</xml_diff>